<commit_message>
New examples and order on charts
</commit_message>
<xml_diff>
--- a/week3/data/AnnotationChart.xlsx
+++ b/week3/data/AnnotationChart.xlsx
@@ -774,445 +774,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Your Work Here'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Internet Sales</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-C7E2-9846-A2DE-1E05049AB046}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="9"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t>1552: When sales</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t> spiked in October</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-C7E2-9846-A2DE-1E05049AB046}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Your Work Here'!$A$2:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>J</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>F</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>M</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>A</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>M</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>J</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>J</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>A</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>S</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>O</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>N</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>D</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Your Work Here'!$B$2:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>355.15</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>284</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>326.77999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>326.33</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>408.25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>514.44000000000005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>541</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>571</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>815.02</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1552.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>815.02</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>815.02</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C7E2-9846-A2DE-1E05049AB046}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="outEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1737086223"/>
-        <c:axId val="1732792927"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1737086223"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1732792927"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1732792927"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1737086223"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
@@ -1844,549 +1405,6 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2597,47 +1615,6 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{599453FD-BF1E-834F-AD90-A03FB1E983D8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3143,7 +2120,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3331,7 +2308,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>